<commit_message>
2/2 Generacion de actas
</commit_message>
<xml_diff>
--- a/php/report/plantilla_acta_recepcion_istg.xlsx
+++ b/php/report/plantilla_acta_recepcion_istg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\InventarioISTGTest\php\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C143C5E4-425B-47DE-B2EA-F7FE4567AC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6299A72-39CE-4C00-9024-2B49D1726507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -653,7 +653,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -784,6 +784,9 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -819,6 +822,24 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -951,7 +972,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="56029"/>
-          <a:ext cx="16394206" cy="1363832"/>
+          <a:ext cx="16421420" cy="1364633"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1340,7 +1361,7 @@
   <dimension ref="A3:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,54 +1422,54 @@
       <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="63"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="64"/>
+    </row>
+    <row r="9" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="63"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-    </row>
-    <row r="9" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="49"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="63"/>
       <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
+      <c r="J9" s="64"/>
     </row>
     <row r="10" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="64"/>
     </row>
     <row r="11" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="58"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="59"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
     </row>
@@ -1484,7 +1505,7 @@
       <c r="I14" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="J14" s="42"/>
+      <c r="J14" s="65"/>
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1499,7 +1520,7 @@
       <c r="G15" s="32"/>
       <c r="H15" s="28"/>
       <c r="I15" s="29"/>
-      <c r="J15" s="44"/>
+      <c r="J15" s="66"/>
       <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1512,7 +1533,7 @@
       <c r="G16" s="32"/>
       <c r="H16" s="28"/>
       <c r="I16" s="29"/>
-      <c r="J16" s="45"/>
+      <c r="J16" s="67"/>
       <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1525,7 +1546,7 @@
       <c r="G17" s="48"/>
       <c r="H17" s="45"/>
       <c r="I17" s="46"/>
-      <c r="J17" s="44"/>
+      <c r="J17" s="66"/>
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1538,7 +1559,7 @@
       <c r="G18" s="46"/>
       <c r="H18" s="45"/>
       <c r="I18" s="45"/>
-      <c r="J18" s="46"/>
+      <c r="J18" s="68"/>
       <c r="K18" s="4"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1547,61 +1568,61 @@
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="59" t="s">
+      <c r="A20" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="60"/>
-      <c r="I20" s="60"/>
-      <c r="J20" s="61"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="62"/>
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="56" t="s">
+      <c r="A21" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="57"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="57"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="58"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="59"/>
     </row>
     <row r="22" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="56" t="s">
+      <c r="A22" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="57"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="57"/>
-      <c r="J22" s="58"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="59"/>
     </row>
     <row r="23" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="56" t="s">
+      <c r="A23" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57"/>
-      <c r="J23" s="58"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="59"/>
     </row>
     <row r="24" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="39"/>
@@ -1616,32 +1637,32 @@
       <c r="J24" s="41"/>
     </row>
     <row r="25" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
-      <c r="J25" s="58"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
+      <c r="J25" s="59"/>
     </row>
     <row r="26" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="56" t="s">
+      <c r="A26" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="57"/>
-      <c r="J26" s="58"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="58"/>
+      <c r="J26" s="59"/>
     </row>
     <row r="27" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
@@ -1688,10 +1709,10 @@
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="53" t="s">
+      <c r="G30" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="H30" s="53"/>
+      <c r="H30" s="54"/>
       <c r="I30" s="9"/>
       <c r="J30" s="19"/>
     </row>
@@ -1717,17 +1738,17 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="20"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="51"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="52"/>
       <c r="D34" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51" t="s">
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="H34" s="51"/>
+      <c r="H34" s="52"/>
       <c r="I34" s="1"/>
       <c r="J34" s="21"/>
     </row>
@@ -1740,8 +1761,8 @@
       <c r="D35" s="38"/>
       <c r="E35" s="35"/>
       <c r="F35" s="35"/>
-      <c r="G35" s="54"/>
-      <c r="H35" s="55"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="56"/>
       <c r="I35" s="1"/>
       <c r="J35" s="21"/>
     </row>
@@ -1752,10 +1773,10 @@
       </c>
       <c r="C36" s="24"/>
       <c r="D36" s="38"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="55"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="56"/>
       <c r="I36" s="1"/>
       <c r="J36" s="21"/>
     </row>
@@ -1767,10 +1788,10 @@
         <v>12</v>
       </c>
       <c r="E37" s="1"/>
-      <c r="G37" s="50" t="s">
+      <c r="G37" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="H37" s="50"/>
+      <c r="H37" s="51"/>
       <c r="J37" s="15"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -1807,7 +1828,7 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A8:J10"/>
+    <mergeCell ref="E9:G9"/>
     <mergeCell ref="G37:H37"/>
     <mergeCell ref="G34:H34"/>
     <mergeCell ref="B34:C34"/>

</xml_diff>